<commit_message>
obtener subpreguntas por pregunta programáticamente + orden repo
</commit_message>
<xml_diff>
--- a/problemas_datos.xlsx
+++ b/problemas_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Pregunta</t>
   </si>
@@ -34,6 +34,30 @@
   </si>
   <si>
     <t>data/output/10044/4275748_p16</t>
+  </si>
+  <si>
+    <t>data/output/10088/4277181</t>
+  </si>
+  <si>
+    <t>N° de subpreguntas incorrecto para estudiante 4277181,                    se encontraron 166 subpreguntas</t>
+  </si>
+  <si>
+    <t>data/output/10121/4278294</t>
+  </si>
+  <si>
+    <t>N° de subpreguntas incorrecto para estudiante 4278294,                    se encontraron 166 subpreguntas</t>
+  </si>
+  <si>
+    <t>data/output/10157/4279607_p20</t>
+  </si>
+  <si>
+    <t>data/output/10157/4279607_p4</t>
+  </si>
+  <si>
+    <t>data/output/10157/4279607</t>
+  </si>
+  <si>
+    <t>N° de subpreguntas incorrecto para estudiante 4279607,                    se encontraron 155 subpreguntas</t>
   </si>
 </sst>
 </file>
@@ -382,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +441,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
modulo generar insumos listo
</commit_message>
<xml_diff>
--- a/problemas_datos.xlsx
+++ b/problemas_datos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,6 +769,66 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\00093\4003684_p_</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Pregunta no pudo ser procesada</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\00206\4007946_p2</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Pregunta no pudo ser procesada</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\00206\4007946_p3</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Pregunta no pudo ser procesada</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\00206\4007946_p26</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Pregunta no pudo ser procesada</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\00206\4007946_p25</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Pregunta no pudo ser procesada</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
mejora manejo nuevo error, parte 2
</commit_message>
<xml_diff>
--- a/problemas_datos.xlsx
+++ b/problemas_datos.xlsx
@@ -1,60 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos_pesaos\repo-simce\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Pregunta</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Nivel</t>
-  </si>
-  <si>
-    <t>data\output\output_subpreg\CE\00199\4000081</t>
-  </si>
-  <si>
-    <t>No existen archivos disponibles para estudiante serie 4000081</t>
-  </si>
-  <si>
-    <t>Estudiante</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -73,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -375,39 +407,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col width="44.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="56.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Pregunta</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nivel</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\CE\00199\4000081</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>No existen archivos disponibles para estudiante serie 4000081</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>data\output\output_subpreg\CE\00200\4000082</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>No existen archivos disponibles para estudiante serie 4000082</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>